<commit_message>
AFDP-2564: Remove description required rule for enter queue
</commit_message>
<xml_diff>
--- a/acm/rules/drools-enter-queue-rules-foia.xlsx
+++ b/acm/rules/drools-enter-queue-rules-foia.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\foia-extension\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dame.gjorgjievski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
   <si>
     <t>RuleSet</t>
   </si>
@@ -259,15 +259,6 @@
   </si>
   <si>
     <t>Request category is required</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>details == null || details?.trim().isEmpty()</t>
-  </si>
-  <si>
-    <t>Description is required</t>
   </si>
   <si>
     <t>expedite flag</t>
@@ -785,7 +776,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5410200</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -828,7 +819,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5410200</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -871,7 +862,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5410200</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1207,22 +1198,22 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.75"/>
-    <col min="2" max="2" width="39.25"/>
-    <col min="3" max="3" width="164.125"/>
-    <col min="4" max="4" width="78.875"/>
-    <col min="5" max="5" width="255.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.125"/>
-    <col min="7" max="7" width="35.625"/>
-    <col min="8" max="1025" width="8.75"/>
+    <col min="1" max="1" width="14.7109375"/>
+    <col min="2" max="2" width="39.28515625"/>
+    <col min="3" max="3" width="164.140625"/>
+    <col min="4" max="4" width="78.85546875"/>
+    <col min="5" max="5" width="255.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625"/>
+    <col min="7" max="7" width="35.5703125"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1293,7 +1284,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1306,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1391,7 +1382,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1486,7 +1477,7 @@
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F23" t="s">
         <v>31</v>
@@ -1501,7 +1492,7 @@
       </c>
       <c r="D24" s="22"/>
       <c r="E24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F24" t="s">
         <v>33</v>
@@ -1516,7 +1507,7 @@
       </c>
       <c r="D25" s="22"/>
       <c r="E25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F25" t="s">
         <v>35</v>
@@ -1531,7 +1522,7 @@
       </c>
       <c r="D26" s="22"/>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F26" t="s">
         <v>37</v>
@@ -1546,7 +1537,7 @@
       </c>
       <c r="D27" s="22"/>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F27" t="s">
         <v>39</v>
@@ -1561,7 +1552,7 @@
       </c>
       <c r="D28" s="22"/>
       <c r="E28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F28" t="s">
         <v>41</v>
@@ -1576,7 +1567,7 @@
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
         <v>43</v>
@@ -1591,7 +1582,7 @@
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
         <v>45</v>
@@ -1606,7 +1597,7 @@
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F31" t="s">
         <v>47</v>
@@ -1621,7 +1612,7 @@
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F32" t="s">
         <v>49</v>
@@ -1636,7 +1627,7 @@
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F33" t="s">
         <v>51</v>
@@ -1736,77 +1727,62 @@
       <c r="B40" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="22"/>
+      <c r="C40" t="s">
+        <v>71</v>
+      </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E41" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F42" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E43" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
         <v>85</v>
-      </c>
-      <c r="C44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1828,7 +1804,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.75"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1847,7 +1823,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.75"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>